<commit_message>
Allow selection of def assay in Module Scoring
</commit_message>
<xml_diff>
--- a/markerGenes.xlsx
+++ b/markerGenes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PYR/juno/work/bic/socci/Work/Users/SchmittA/ShamsedA/Proj_11206/Seurate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PYR/juno/work/bic/socci/Work/Users/SchmittA/ShamsedA/Proj_11206/Seurate/AddPclaf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB60AAE8-FB5E-8E4D-A248-D4BF52966297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2C8E1C-3925-B048-9752-3D5A8974A505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9500" yWindow="7500" windowWidth="27640" windowHeight="16140" xr2:uid="{D57583E5-575D-9645-B6C9-7C35A91A79A3}"/>
   </bookViews>
@@ -87,10 +87,10 @@
     <t>T Cells</t>
   </si>
   <si>
-    <t>CD163, XD86, CD80, CD68, CD74, CD14</t>
-  </si>
-  <si>
     <t>CD79A, CD79B, CD19</t>
+  </si>
+  <si>
+    <t>CD163, CD86, CD80, CD68, CD74, CD14</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -553,7 +553,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>